<commit_message>
bug fixed (showing same bank twice in summary)
</commit_message>
<xml_diff>
--- a/assets/other/dummy_summary_data.xlsx
+++ b/assets/other/dummy_summary_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Alpha Aces\Projects\Bank_Statemants_Automation\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CD38B5-8EDB-44CC-92C9-24930B5A37A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC5C606-A545-424D-85B4-E8FA8FE06E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,15 +28,6 @@
     <t>Bank</t>
   </si>
   <si>
-    <t>Start_Date</t>
-  </si>
-  <si>
-    <t>End_Date</t>
-  </si>
-  <si>
-    <t>Pending_days</t>
-  </si>
-  <si>
     <t>Transactions</t>
   </si>
   <si>
@@ -65,6 +56,15 @@
   </si>
   <si>
     <t>John Doe</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Pending days</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,24 +459,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>45472</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>45657</v>
@@ -513,10 +513,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>45292</v>
@@ -533,10 +533,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>45536</v>
@@ -553,10 +553,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>45501</v>
@@ -573,10 +573,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>44928</v>
@@ -593,10 +593,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>43557</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2">
         <v>45640</v>

</xml_diff>